<commit_message>
Add second repository to input
</commit_message>
<xml_diff>
--- a/input/repos.xlsx
+++ b/input/repos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8a7119f9a48e1aa7/Cursor/JiraFlowEval/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="11_2B59D2BFD380D14AEF0D7B32443088B35299F3AE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D29E23BA-8C2D-4411-B6E4-5A9835F61432}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="11_2B59D2BFD380D14AEF0D7B32443088B35299F3AE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{80C09D8B-44CE-405C-B80B-B02D5008B066}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,15 +31,6 @@
     <t>email</t>
   </si>
   <si>
-    <t>https://github.com/example/data-pipeline-2</t>
-  </si>
-  <si>
-    <t>Bob</t>
-  </si>
-  <si>
-    <t>bob@example.com</t>
-  </si>
-  <si>
     <t>https://github.com/danielhantunes/JiraFlow</t>
   </si>
   <si>
@@ -47,6 +38,15 @@
   </si>
   <si>
     <t>danielh.engenhariadesistemas@gmail.com</t>
+  </si>
+  <si>
+    <t>https://github.com/danielhantunes/jiraflow-sample1</t>
+  </si>
+  <si>
+    <t>Joao</t>
+  </si>
+  <si>
+    <t>email@example.com</t>
   </si>
 </sst>
 </file>
@@ -423,7 +423,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -445,30 +445,32 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>3</v>
+      <c r="A3" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{3E97C23D-40D0-4620-A5FF-AEBB0472D40D}"/>
     <hyperlink ref="C2" r:id="rId2" xr:uid="{00337001-EFDD-43D3-963F-C9BD1021468D}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{4018C69D-5B7C-4DED-B6D5-AE349D6D7C5F}"/>
+    <hyperlink ref="C3" r:id="rId4" xr:uid="{0328946D-EA2E-448B-8C70-6CF3F5465D22}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add repo to repos list
</commit_message>
<xml_diff>
--- a/input/repos.xlsx
+++ b/input/repos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8a7119f9a48e1aa7/Cursor/JiraFlowEval/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="11_2B59D2BFD380D14AEF0D7B32443088B35299F3AE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{80C09D8B-44CE-405C-B80B-B02D5008B066}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="11_2B59D2BFD380D14AEF0D7B32443088B35299F3AE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8DCC61D1-08CA-4056-9A86-B89AE84DD16D}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>repo_url</t>
   </si>
@@ -47,6 +47,12 @@
   </si>
   <si>
     <t>email@example.com</t>
+  </si>
+  <si>
+    <t>https://github.com/repoaleatorio/repoaleatorio</t>
+  </si>
+  <si>
+    <t>maria</t>
   </si>
 </sst>
 </file>
@@ -420,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -465,12 +471,25 @@
         <v>8</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{3E97C23D-40D0-4620-A5FF-AEBB0472D40D}"/>
     <hyperlink ref="C2" r:id="rId2" xr:uid="{00337001-EFDD-43D3-963F-C9BD1021468D}"/>
     <hyperlink ref="A3" r:id="rId3" xr:uid="{4018C69D-5B7C-4DED-B6D5-AE349D6D7C5F}"/>
     <hyperlink ref="C3" r:id="rId4" xr:uid="{0328946D-EA2E-448B-8C70-6CF3F5465D22}"/>
+    <hyperlink ref="A4" r:id="rId5" xr:uid="{8208039D-748E-457C-9878-7A2E4ED1C915}"/>
+    <hyperlink ref="C4" r:id="rId6" xr:uid="{075320B4-7C05-4838-B87F-B0D8311BBCDA}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>